<commit_message>
Cleaned up and finally corrected the Label-Errors
</commit_message>
<xml_diff>
--- a/variable-selection/soep-feature-selection-xls.xlsx
+++ b/variable-selection/soep-feature-selection-xls.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="32980" windowHeight="17100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="6520" windowWidth="28800" windowHeight="16500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pdatensatz" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -2427,10 +2427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H118"/>
+  <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="118" workbookViewId="0">
-      <selection activeCell="G109" sqref="G109"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="118" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5479,6 +5479,12 @@
         <v>680</v>
       </c>
     </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D119">
+        <f>117-25</f>
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>